<commit_message>
12.31 lab to home
</commit_message>
<xml_diff>
--- a/spModle.xlsx
+++ b/spModle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KMS_Workstation\Desktop\excelize_json_practice\excelize_json_practice\PI_SP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0869E12F-65F6-41CD-BFD0-E919AA94F7C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B63119B8-B949-4ADB-9396-F1ABD34E15AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3901,8 +3901,8 @@
   </sheetPr>
   <dimension ref="A1:AZ993"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P31" workbookViewId="0">
-      <selection activeCell="AU47" sqref="AU47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30:X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -6256,63 +6256,33 @@
       <c r="B37" s="69"/>
       <c r="C37" s="70"/>
       <c r="D37" s="71"/>
-      <c r="E37" s="72">
-        <v>1</v>
-      </c>
-      <c r="F37" s="72">
-        <v>1</v>
-      </c>
+      <c r="E37" s="72"/>
+      <c r="F37" s="72"/>
       <c r="G37" s="73"/>
-      <c r="H37" s="74">
-        <v>1600</v>
-      </c>
-      <c r="I37" s="74">
+      <c r="H37" s="74"/>
+      <c r="I37" s="74"/>
+      <c r="J37" s="75"/>
+      <c r="K37" s="76">
+        <f t="shared" ref="K37:K40" si="0">H37+I37+J37</f>
         <v>0</v>
       </c>
-      <c r="J37" s="75">
+      <c r="L37" s="77"/>
+      <c r="M37" s="72"/>
+      <c r="N37" s="78"/>
+      <c r="O37" s="79">
+        <f>U37+V37+W37+X37</f>
         <v>0</v>
-      </c>
-      <c r="K37" s="76">
-        <f t="shared" ref="K37:K40" si="0">H37+I37+J37</f>
-        <v>1600</v>
-      </c>
-      <c r="L37" s="77">
-        <v>0</v>
-      </c>
-      <c r="M37" s="72">
-        <v>0</v>
-      </c>
-      <c r="N37" s="78">
-        <v>0</v>
-      </c>
-      <c r="O37" s="79">
-        <f t="shared" ref="O37:O40" si="1">U37+V37+W37+X37</f>
-        <v>85</v>
       </c>
       <c r="P37" s="79"/>
       <c r="Q37" s="80"/>
-      <c r="R37" s="222" t="e">
-        <f>#REF!*1000</f>
-        <v>#REF!</v>
-      </c>
+      <c r="R37" s="222"/>
       <c r="S37" s="201"/>
       <c r="T37" s="81"/>
-      <c r="U37" s="74">
-        <v>0</v>
-      </c>
-      <c r="V37" s="74">
-        <v>0</v>
-      </c>
-      <c r="W37" s="74">
-        <v>45</v>
-      </c>
-      <c r="X37" s="82">
-        <v>40</v>
-      </c>
-      <c r="Y37" s="83">
-        <f t="shared" ref="Y37:Y40" si="2">(K37+O37)-J37</f>
-        <v>1685</v>
-      </c>
+      <c r="U37" s="74"/>
+      <c r="V37" s="74"/>
+      <c r="W37" s="74"/>
+      <c r="X37" s="82"/>
+      <c r="Y37" s="83"/>
       <c r="Z37" s="84"/>
       <c r="AA37" s="84"/>
       <c r="AB37" s="84"/>
@@ -6346,63 +6316,33 @@
       <c r="B38" s="69"/>
       <c r="C38" s="70"/>
       <c r="D38" s="71"/>
-      <c r="E38" s="72">
-        <v>1</v>
-      </c>
-      <c r="F38" s="72">
-        <v>1</v>
-      </c>
+      <c r="E38" s="72"/>
+      <c r="F38" s="72"/>
       <c r="G38" s="73"/>
-      <c r="H38" s="74">
-        <v>1600</v>
-      </c>
-      <c r="I38" s="74">
+      <c r="H38" s="74"/>
+      <c r="I38" s="74"/>
+      <c r="J38" s="75"/>
+      <c r="K38" s="76">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J38" s="75">
+      <c r="L38" s="77"/>
+      <c r="M38" s="72"/>
+      <c r="N38" s="78"/>
+      <c r="O38" s="79">
+        <f t="shared" ref="O38:O40" si="1">U38+V38+W38+X38</f>
         <v>0</v>
-      </c>
-      <c r="K38" s="76">
-        <f t="shared" si="0"/>
-        <v>1600</v>
-      </c>
-      <c r="L38" s="77">
-        <v>0</v>
-      </c>
-      <c r="M38" s="72">
-        <v>0</v>
-      </c>
-      <c r="N38" s="78">
-        <v>0</v>
-      </c>
-      <c r="O38" s="79">
-        <f t="shared" si="1"/>
-        <v>100</v>
       </c>
       <c r="P38" s="79"/>
       <c r="Q38" s="80"/>
-      <c r="R38" s="222" t="e">
-        <f>#REF!*1000</f>
-        <v>#REF!</v>
-      </c>
+      <c r="R38" s="222"/>
       <c r="S38" s="201"/>
       <c r="T38" s="81"/>
-      <c r="U38" s="74">
-        <v>0</v>
-      </c>
-      <c r="V38" s="74">
-        <v>0</v>
-      </c>
-      <c r="W38" s="74">
-        <v>45</v>
-      </c>
-      <c r="X38" s="82">
-        <v>55</v>
-      </c>
-      <c r="Y38" s="83">
-        <f t="shared" si="2"/>
-        <v>1700</v>
-      </c>
+      <c r="U38" s="74"/>
+      <c r="V38" s="74"/>
+      <c r="W38" s="74"/>
+      <c r="X38" s="82"/>
+      <c r="Y38" s="83"/>
       <c r="Z38" s="84"/>
       <c r="AA38" s="84"/>
       <c r="AB38" s="84"/>
@@ -6436,63 +6376,33 @@
       <c r="B39" s="69"/>
       <c r="C39" s="70"/>
       <c r="D39" s="71"/>
-      <c r="E39" s="72">
-        <v>1</v>
-      </c>
-      <c r="F39" s="72">
-        <v>1</v>
-      </c>
+      <c r="E39" s="72"/>
+      <c r="F39" s="72"/>
       <c r="G39" s="73"/>
-      <c r="H39" s="74">
-        <v>1720</v>
-      </c>
-      <c r="I39" s="74">
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="76">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J39" s="75">
-        <v>0</v>
-      </c>
-      <c r="K39" s="76">
-        <f t="shared" si="0"/>
-        <v>1720</v>
-      </c>
-      <c r="L39" s="77">
-        <v>0</v>
-      </c>
-      <c r="M39" s="72">
-        <v>0</v>
-      </c>
-      <c r="N39" s="78">
-        <v>0</v>
-      </c>
+      <c r="L39" s="77"/>
+      <c r="M39" s="72"/>
+      <c r="N39" s="78"/>
       <c r="O39" s="79">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="P39" s="79"/>
       <c r="Q39" s="80"/>
-      <c r="R39" s="222" t="e">
-        <f>#REF!*1000</f>
-        <v>#REF!</v>
-      </c>
+      <c r="R39" s="222"/>
       <c r="S39" s="201"/>
       <c r="T39" s="81"/>
-      <c r="U39" s="74">
-        <v>0</v>
-      </c>
-      <c r="V39" s="74">
-        <v>0</v>
-      </c>
-      <c r="W39" s="74">
-        <v>0</v>
-      </c>
-      <c r="X39" s="82">
-        <v>60</v>
-      </c>
-      <c r="Y39" s="83">
-        <f t="shared" si="2"/>
-        <v>1780</v>
-      </c>
+      <c r="U39" s="74"/>
+      <c r="V39" s="74"/>
+      <c r="W39" s="74"/>
+      <c r="X39" s="82"/>
+      <c r="Y39" s="83"/>
       <c r="Z39" s="84"/>
       <c r="AA39" s="84"/>
       <c r="AB39" s="84"/>
@@ -6526,63 +6436,33 @@
       <c r="B40" s="69"/>
       <c r="C40" s="70"/>
       <c r="D40" s="71"/>
-      <c r="E40" s="72">
-        <v>1</v>
-      </c>
-      <c r="F40" s="72">
-        <v>1</v>
-      </c>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
       <c r="G40" s="73"/>
-      <c r="H40" s="74">
-        <v>1605</v>
-      </c>
-      <c r="I40" s="74">
+      <c r="H40" s="74"/>
+      <c r="I40" s="74"/>
+      <c r="J40" s="75"/>
+      <c r="K40" s="76">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="75">
-        <v>0</v>
-      </c>
-      <c r="K40" s="76">
-        <f t="shared" si="0"/>
-        <v>1605</v>
-      </c>
-      <c r="L40" s="77">
-        <v>0</v>
-      </c>
-      <c r="M40" s="72">
-        <v>0</v>
-      </c>
-      <c r="N40" s="78">
-        <v>0</v>
-      </c>
+      <c r="L40" s="77"/>
+      <c r="M40" s="72"/>
+      <c r="N40" s="78"/>
       <c r="O40" s="79">
         <f t="shared" si="1"/>
-        <v>140</v>
+        <v>0</v>
       </c>
       <c r="P40" s="79"/>
       <c r="Q40" s="80"/>
-      <c r="R40" s="222" t="e">
-        <f>#REF!*1000</f>
-        <v>#REF!</v>
-      </c>
+      <c r="R40" s="222"/>
       <c r="S40" s="201"/>
       <c r="T40" s="81"/>
-      <c r="U40" s="74">
-        <v>0</v>
-      </c>
-      <c r="V40" s="74">
-        <v>45</v>
-      </c>
-      <c r="W40" s="74">
-        <v>55</v>
-      </c>
-      <c r="X40" s="82">
-        <v>40</v>
-      </c>
-      <c r="Y40" s="83">
-        <f t="shared" si="2"/>
-        <v>1745</v>
-      </c>
+      <c r="U40" s="74"/>
+      <c r="V40" s="74"/>
+      <c r="W40" s="74"/>
+      <c r="X40" s="82"/>
+      <c r="Y40" s="83"/>
       <c r="Z40" s="84"/>
       <c r="AA40" s="84"/>
       <c r="AB40" s="84"/>
@@ -58394,7 +58274,7 @@
     <mergeCell ref="E8:G8"/>
   </mergeCells>
   <phoneticPr fontId="73" type="noConversion"/>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="選擇銀行" sqref="S4 Y4" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"華銀,一銀,上海銀,板信,彰化銀,兆豐"</formula1>
     </dataValidation>

</xml_diff>